<commit_message>
correct upsert simple built gpu
</commit_message>
<xml_diff>
--- a/apps/pczone/test/support/data/products.xlsx
+++ b/apps/pczone/test/support/data/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achilles/Projects/pczone_umbrella/apps/pc_zone/test/support/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achilles/Projects/pczone_umbrella/apps/pczone/test/support/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E8A97C-39AA-F740-A82A-E09D5F1482F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE4BA36-1BEA-C444-B4CF-23F5E8D39D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2461082F-601B-E94F-AE09-008E6CBA7E88}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>kind</t>
   </si>
@@ -262,6 +262,51 @@
   </si>
   <si>
     <t>1tb-samsung-860-evo/100%</t>
+  </si>
+  <si>
+    <t>i3-9100</t>
+  </si>
+  <si>
+    <t>i3-9100/tray</t>
+  </si>
+  <si>
+    <t>i3-9100T</t>
+  </si>
+  <si>
+    <t>i3-9100t/tray</t>
+  </si>
+  <si>
+    <t>i3-9100F</t>
+  </si>
+  <si>
+    <t>i3-9100f/tray</t>
+  </si>
+  <si>
+    <t>dell-optiplex-7060-sff</t>
+  </si>
+  <si>
+    <t>dell-optiplex-7060-sff/used</t>
+  </si>
+  <si>
+    <t>gpu</t>
+  </si>
+  <si>
+    <t>nvidia-quadro-k600</t>
+  </si>
+  <si>
+    <t>nvidia-quadro-k600/used</t>
+  </si>
+  <si>
+    <t>4gb-dimm-ddr4-2666-mixed</t>
+  </si>
+  <si>
+    <t>8gb-dimm-ddr4-2666-mixed</t>
+  </si>
+  <si>
+    <t>4gb-dimm-ddr4-2666-mixed/used</t>
+  </si>
+  <si>
+    <t>8gb-dimm-ddr4-2666-mixed/used</t>
   </si>
 </sst>
 </file>
@@ -631,7 +676,7 @@
   <dimension ref="A1:I147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +687,7 @@
     <col min="4" max="4" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
   </cols>
@@ -1426,6 +1471,167 @@
         <v>2000000</v>
       </c>
       <c r="G34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2200000</v>
+      </c>
+      <c r="G35" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="2">
+        <v>3000000</v>
+      </c>
+      <c r="G36" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="G37" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1850000</v>
+      </c>
+      <c r="G38" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="2">
+        <v>600000</v>
+      </c>
+      <c r="G39" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="2">
+        <v>340000</v>
+      </c>
+      <c r="G40" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="2">
+        <v>680000</v>
+      </c>
+      <c r="G41" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>